<commit_message>
começando o web-scraping para pegar os dados dos reus sem ADV
</commit_message>
<xml_diff>
--- a/Processos.xlsx
+++ b/Processos.xlsx
@@ -14,12 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="217">
+  <si>
+    <t>Processo</t>
+  </si>
+  <si>
+    <t>Participantes</t>
+  </si>
   <si>
     <t>Processo Nº ATOrd-0001590-49.2013.5.03.0001 $$ 10625</t>
   </si>
   <si>
-    <t>--------------------------------------------------------------------------------</t>
+    <t>Processo----------------------------------------------------------------------</t>
   </si>
   <si>
     <t>Processo Nº ATOrd-0010294-43.2016.5.03.0002 $$ 11565</t>
@@ -164,6 +170,9 @@
   </si>
   <si>
     <t xml:space="preserve">INTERESSADOMARCO ANTONIO BARBOSA OLIVEIRA JUNIOR   </t>
+  </si>
+  <si>
+    <t>Participantes----------------------------------------------------------------------</t>
   </si>
   <si>
     <t xml:space="preserve">AUTOR JOSE VENCESLAU CIRIACO </t>
@@ -1020,1875 +1029,1875 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B52" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B53" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B54" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B55" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B56" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B57" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B60" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B61" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B62" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B63" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B64" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B65" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B66" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B67" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B68" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B69" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B70" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B71" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B72" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B73" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B74" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B75" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B76" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B77" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B78" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B79" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B80" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B81" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B82" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B83" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B84" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B85" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B86" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B87" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B88" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B89" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B90" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B91" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B92" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B93" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B94" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B95" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B96" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B97" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B98" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B99" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B100" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B101" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B102" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B103" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B104" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B105" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B106" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B107" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B108" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B109" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B110" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B111" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B112" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B113" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B114" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B115" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B116" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B117" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B118" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B119" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B120" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B121" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B122" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B123" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B124" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B125" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B126" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B127" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B128" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B129" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B130" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B131" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B132" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B133" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B134" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B135" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B136" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B137" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B138" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B139" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B140" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B141" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B142" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B143" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B144" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B145" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B146" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B147" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B148" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B149" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B150" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B151" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B152" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B153" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B154" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B155" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B156" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B157" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B158" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B159" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B160" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B161" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B162" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B163" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B164" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B165" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B166" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B167" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B168" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B169" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B170" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B171" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B172" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B173" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B174" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B175" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B176" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B177" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B178" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B179" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B180" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B181" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B182" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B183" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B184" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B185" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B186" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B187" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B188" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B189" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B190" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B191" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B192" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B193" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B194" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B195" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B196" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B197" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B198" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B199" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B200" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B201" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B202" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B203" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B204" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B205" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B206" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B207" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B208" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B209" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B210" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B211" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B212" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B213" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B214" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B215" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B216" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="217" spans="1:2">
       <c r="A217" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B217" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B218" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="219" spans="1:2">
       <c r="A219" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B219" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B220" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="221" spans="1:2">
       <c r="A221" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B221" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="222" spans="1:2">
       <c r="A222" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B222" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="223" spans="1:2">
       <c r="A223" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B223" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B224" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B225" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B226" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B227" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B228" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B229" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B230" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="231" spans="1:2">
       <c r="A231" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B231" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B232" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="233" spans="1:2">
       <c r="A233" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B233" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B234" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
web scraping pegando info pessoas sem homonimo e somente pessoas fisicas
</commit_message>
<xml_diff>
--- a/Processos.xlsx
+++ b/Processos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="454">
   <si>
     <t>Processo</t>
   </si>
@@ -151,6 +151,141 @@
     <t>Processo Nº ATOrd-0010750-71.2018.5.03.0018 $$ 110167</t>
   </si>
   <si>
+    <t>Processo Nº ATOrd-0010154-14.2023.5.03.0018 $$ 112514</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010806-67.2022.5.03.0179 $$ 112840</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010175-87.2023.5.03.0018 $$ 113548</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010173-20.2023.5.03.0018 $$ 113623</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010170-65.2023.5.03.0018 $$ 113770</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010178-42.2023.5.03.0018 $$ 114046</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0156100-73.2007.5.03.0019 $$ 116148</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0163400-18.2009.5.03.0019 $$ 116230</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0000975-10.2010.5.03.0019 $$ 120005</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0001978-60.2011.5.03.0020 $$ 120525</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0120100-28.1994.5.03.0020 $$ 120739</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010179-21.2023.5.03.0020 $$ 120912</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0000317-04.2015.5.03.0021 $$ 121463</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010048-43.2023.5.03.0021 $$ 123353</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010400-40.2019.5.03.0021 $$ 126649</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010103-91.2023.5.03.0021 $$ 130126</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010172-14.2023.5.03.0025 $$ 133746</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010156-93.2023.5.03.0111 $$ 140545</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010192-08.2023.5.03.0024 $$ 141299</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010115-93.2023.5.03.0025 $$ 148619</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0000951-22.2014.5.03.0025 $$ 153357</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010643-23.2019.5.03.0105 $$ 168326</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010126-54.2015.5.03.0106 $$ 170747</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010193-38.2023.5.03.0106 $$ 171320</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0000528-13.2014.5.03.0106 $$ 174113</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010869-22.2019.5.03.0107 $$ 174692</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010040-96.2023.5.03.0108 $$ 174777</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010025-30.2023.5.03.0108 $$ 174803</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010175-24.2023.5.03.0136 $$ 176120</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010178-60.2023.5.03.0109 $$ 177586</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0011011-15.2022.5.03.0109 $$ 183159</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010015-80.2023.5.03.0109 $$ 185133</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0030700-75.2004.5.03.0109 $$ 185752</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0002303-59.2011.5.03.0109 $$ 186037</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010710-44.2017.5.03.0109 $$ 187180</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010505-07.2020.5.03.0110 $$ 188544</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0000100-87.2012.5.03.0110 $$ 189204</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010171-65.2023.5.03.0110 $$ 189878</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010181-09.2023.5.03.0111 $$ 194883</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010180-24.2023.5.03.0111 $$ 194973</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010608-37.2022.5.03.0112 $$ 195218</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010187-13.2023.5.03.0112 $$ 196174</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010188-95.2023.5.03.0112 $$ 197343</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010731-32.2022.5.03.0113 $$ 198292</t>
+  </si>
+  <si>
+    <t>Processo Nº ATOrd-0010190-62.2023.5.03.0113AUTOR GLEISON ANGELO DOMINGUES DE $$ 199005</t>
+  </si>
+  <si>
     <t xml:space="preserve">AUTOR LEANDRO SOUZA GOMES </t>
   </si>
   <si>
@@ -665,6 +800,582 @@
   </si>
   <si>
     <t xml:space="preserve">INTERESSADOINSTITUTO NACIONAL DE PREVIDÊNCIA SOCIAL (INSS)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR ARI ELISEI VILELA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO RENATO VICTOR AMARAL(OAB: 316922/SP) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU CAPGEMINI BRASIL S/A   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR MIQUELINE DO NASCIMENTO VARELA NEVES </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO CLAUDIA PEIXOTO DE AZEVEDO SILVA(OAB: 159402/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU ROBERT ZANANDREIZ DE MATTOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU J.M SERVICOS AEREOS LTDA - ME </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU GUSTAVO ALVES SOARES </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU CONCEICAO ROSA DA SILVA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU MARCUS LEANDRO LOPES DA SILVA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU CONSTRUTORA ALVES LTDA. - EPP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU PHILLIP MATIAS ZANANDREIZ SALAZAR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU ANDRE FILIPE CARVALHO MATTOS   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR JEFFERSON LUIZ FREIRE SILVA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO DIANA CLAUDINO EUSTAQUIO(OAB: 156262/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU INFRAREDES - INFRAESTRUTURA E REDES DE TELECOMUNICACOES LTDA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU CLARO S.A.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR VANIA MENDES PIRES </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU ACAO CONTACT CENTER EIRELI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU BANCO LOSANGO S.A. - BANCO MULTIPLO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU BANCO BRADESCO S.A.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR BARBARA TAIS MORAIS ALVES </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO ALFRED GIMPEL MOREIRA PINTO(OAB: 217884/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU CEDOC - GESTAO DE DOCUMENTOS, ARQUIVOS E INFORMACOES LTDA   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR ICARO GABRIEL FERREIRA DE SOUZA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO BRENO HAROLDO RIBEIRO DE OLIVEIRA(OAB: 134890/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU ALEXANDRE HERMENEGILDO MATEUS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU ARTE CRIAR MOVEIS E INTERIORES LTDA   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR MIGUEL ALVES COSTA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO ALOIZIO JOSE DE CARVALHO(OAB: 46462/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU VICENTE DOROTEU DOS SANTOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU ATLAN SERVICOS LTDA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU TIAGO GLICERIO DOS SANTOS   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR GENIVAL MANOEL DOS SANTOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO JOSE GUMERCINDO VILELA(OAB: 45351/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU LAR MINAS ENGENHARIA LTDA - EPP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU LEANDRO ATILIO RODRIGUES   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR CLAUDIO DA SILVA ALMEIDA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO PAULO SANDERSON GIL NUNES(OAB: 38562/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU ADERLAINE AUGUSTA DE OLIVEIRA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU MARIA LUIZA DA CONCEICAO OLIVEIRA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU INICIATIVA EMPREENDIMENTOS E SERVICOS LTDA   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR MARCELINO BATISTA DA SILVA Código para aferir autenticidade deste caderno: 1972303681/2023 Tribunal Regional do Trabalho da 3ª Região 3360 Data da Disponibilização: Segunda-feira, 13 de Março de 2023   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO SAMUEL SILVA FONSECA(OAB: 129986/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU RRJ TRANSPORTE DE VALORES, SEGURANCA E VIGILANCIA LTDA. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU TRANSSAFE TRANSPORTE DE VALORES E SEGURANCA PATRIMONIAL LTDA - ME </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU EMBRAFORTE SEGURANCA E TRANSPORTE DE VALORES LTDA. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU MARCOS FELIPE GONCALVES DE VILHENA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU MARCOS ANDRE PAES DE VILHENA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU PEDRO HENRIQUE GONCALVES DE VILHENA TERCEIRO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTERESSADODETRAN SP   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR MARIA GUEDES DA LUZ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO FELIPE MAURICIO SALIBA DE SOUZA(OAB: 108211/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU SILVIO BUFONI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU CARLOS JORGE MOREIRA DE SOUZA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU ROGERIO DE CARVALHO NOGUEIRA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU RIOFORTE SERVICOS TECNICOS S/A TERCEIRO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTERESSADOServiço Registral do 11º Ofício de Registro de Imóveis   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR LEONARDO HENRIQUE DA SILVA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU S.E.S. SISTEMAS ELETRONICOS LTDA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU PLANTAO SERVICOS DE VIGILANCIA LTDA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU CONSERVO SERVICOS GERAIS LTDA   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR THAIS DE MELO FRANCO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO Alisson Wagner Ferreira(OAB: 113363/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU MASTER BRASIL S.A.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR DANIEL LAURISTON DA CUNHA PEREIRA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO EDUARDO HENRIQUE DA SILVA CASTRO(OAB: 108893/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU TURILESSA LTDA   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR SILVIA OLIVEIRA MOTIN INACIO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO MARCOS AURELIO ROCHA PEREIRA DORNELAS(OAB: 167926/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU MUNICIPIO DE BELO HORIZONTE TERCEIRO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR BARBARA CRISTINA ZUBA SOARES </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO Rosemberg Chaefer Nascimento Silva(OAB: 109135/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU PATRICIA VALERIO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU RIO ZONA SUL CLINICA ODONTOLOGICA LTDA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU MARCELO FERREIRA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU RODRIGO VALERIO COSTA PEDRO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU RIZZO CLINICA ODONTOLOGICA LTDA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU LUIZ RAFAEL CAMPOS MAGALHAES </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU LOCKE SERVICOS ODONTOLOGICOS LTDA. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU SAVOY SERVICOS DE DIAGNOSTICOS LTDA. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU PW INSTITUTO DE ODONTOLOGIA LTDA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU DANIELLE PENA DUARTE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU ATLAS FRANQUIAS EIRELI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU TECNOLOGIA E ARTE PROTESE ODONTOLOGICA LTDA - EPP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU SERVE MINAS SERVICOS GERAIS LTDA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU PAULO HENRIQUE RODRIGUES </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU EUGENIO JORGE FERREIRA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU BMVF FRANCHISING E PARTICIPACOES LTDA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU RENATO COSTA FRANCO BALDAN   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR SIDNEI DELFINO DOS SANTOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO JANAINA OLIVIA CASTELAR DE PAULA(OAB: 117969/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU VLI MULTIMODAL S.A. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU FERROVIA CENTRO-ATLANTICA S.A  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR CAMILA JARDIM GONCALVES DOS SANTOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO ISABELLA SANGLARD PIMENTA MACHADO(OAB: 104778/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR VIVIANE MARIA COSTA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR ERNANE EUSTAQUIO DOS SANTOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO FELIPE CAMPOS MUZZI(OAB: 111498/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU ULTRA INFINITY TRANSPORTES EIRELI   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR FRANCISCO DE ASSIS ALMEIDA NUNES </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU IPEC - INDUSTRIA DE PERFUMES E COSMETICOS LTDA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU L.A.M. PERFUMES E COSMETICOS LTDA - EPP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU LEOPOLDO MESQUITA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO MARCOS JOSE RODRIGUES(OAB: 57915/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU SOFCON - SOCIEDADE FRANCHISING &amp; CONSULTORIA LTDA. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU MILLENNIUM - COMERCIO DE PERFUMES LTDA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU MARLENE GEISA VILLANI MESQUITA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU MIRTES NASCIMENTO BARBOSA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU LEOPOLDO MESQUITA FILHO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PERITO MIGUEL FERNANDO BARBOSA SILVA TERCEIRO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR MARIA GERALDA DA SILVA MARTINS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO MARCOS AURELIO ROCHA PEREIRA DORNELAS(OAB: 167926/MG) Código para aferir autenticidade deste caderno: 1972303681/2023 Tribunal Regional do Trabalho da 3ª Região 3884 Data da Disponibilização: Segunda-feira, 13 de Março de 2023   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR LORENNA MEIRA DE ALVARENGA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO AIRTON DELCIO ELER JUNIOR(OAB: 108606/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU PAULO GUILHERME ALVARES </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU BIG-GRANDES IDEIAS LTDA TERCEIRO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTERESSADOCARTÓRIO DE REGISTRO DE IMÓVEIS DE ITABIRITO MG ARREMATANTE MARCO ANTONIO ANDERE TEIXEIRA   </t>
+  </si>
+  <si>
+    <t>AUTOR HELEN CRISTINA VIEIRA DE ASSIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR ANTONIO TEIXEIRA BERTANI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO BRUNO ROBERTO PRATES SILVA(OAB: 140500/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU RANAEL SERVICOS EIRELI - ME </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR JULIO CESAR DOS SANTOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO DARLENE MORAIS ASFORA(OAB: 62510/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR DEIVID BAUER GONCALVES </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO RUBEM RIBEIRO NETO(OAB: 118475/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU SETELOC LTDA - ME   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR FERNANDO FERREIRA PIMENTA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO BRUNO VINICIUS DOS SANTOS(OAB: 193197/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU TUPI REBOQUE E TRANSPORTES LTDA   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR KILDARE GODINHO DE SA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO LEONARDO DAVID BRAGA DOS SANTOS(OAB: 149502/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR VANDERLI GOMES DA SILVA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO ATILA ANERES DA SILVA(OAB: 64934/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU BR MINERAIS COMERCIO DE PRODUTOS E EXTRACAO MINERAL LTDA   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR LUCILENE DOS SANTOS CRUZ RODRIGUES </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO ANTONIO RAIMUNDO DE CASTRO QUEIROZ JUNIOR(OAB: 94392/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU TURQUEZA TECIDOS E VESTUARIOS S/A   Código para aferir autenticidade deste caderno: 1972303681/2023 Tribunal Regional do Trabalho da 3ª Região 4042 Data da Disponibilização: Segunda-feira, 13 de Março de 2023   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR PAULO ROBERTO CARAM PATRUS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO FREDERICO POLTRONIERI ANDRADE CRUZ(OAB: 150601/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU CAIXA ECONOMICA FEDERAL   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR ELISANGELA MARIA DE JESUS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO ROBERTO BARRA(OAB: 47868/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU MARIA GENY UTSCH DE CASTRO ARAUJO   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR ELIZETE LELIS DE OLIVEIRA FELIX </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO ARI DE ALMEIDA FILHO(OAB: 25950/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU JOELMA DUARTE DE OLIVEIRA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU UNIVERSO SERVICOS E ASSESSORIA EMPRESARIAL LTDA   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR MARILIA DOS SANTOS DE SOUZA PAULA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO DANILO FELICIO GONÇALVES FERREIRA(OAB: 108729/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU JOSE ARISTON MACHADO SANTIAGO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU HELOISA MACHADO SANTIAGO TERCEIRO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTERESSADOVISA DO BRASIL EMPREENDIMENTOS LTDA TERCEIRO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTERESSADOITAU UNIBANCO S.A. TERCEIRO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTERESSADOAMERICAN EXPRESS BRASIL ASSESSORIA EMPRESARIAL LTDA. TERCEIRO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTERESSADOMASTERCARD BRASIL LTDA TERCEIRO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTERESSADOBANCO CREDICARD S.A. TERCEIRO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTERESSADOBANCO BRADESCO S.A.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR CARLOS EDUARDO DA SILVA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO BRUNO EDUARDO MARTINS TAVARES(OAB: 118883/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU MUNICIPIO DE BELO HORIZONTE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PERITO LEONARDO ROSSI   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR MARIA DE FATIMA XAVIER </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU MINAS FORTE SEGURANCA E VIGILANCIA LTDA   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR VIRGINIA DIAS DE SOUZA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR MAGNO LUIZ VENANCIO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO SAULO MOREIRA GROSSI(OAB: 106437/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU ROUXINOL VIAGENS E TURISMO LTDA   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR DEILSON SOUZA DE OLIVEIRA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO SAMUEL DIAS DE MOURA(OAB: 168718/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU BANCO DO BRASIL SA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU FORTEBANCO VIGILANCIA E SEGURANCA LTDA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU BANCO BRADESCO S.A. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU VANESSA AVELINO VIEIRA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU LAURENCE GUSTAVO PINTO NETO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU TECNOLOGIA BANCARIA S.A. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU FIDELYS SEGURANCA PRIVADA E TRANSPORTE DE VALORES LTDA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU EDSON PINTO NETO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU FORTEBANCO ADMINISTRACAO DE SERVICOS LTDA   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR VALDIVINA RODRIGUES NUNES </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU ARIANE APARECIDA DE OLIVEIRA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU MARIA APARECIDA CRUZ   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR WARLEY BATISTA DE CARVALHO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU ANJOS DA GUARDA SEGURANCA E VIGILANCIA LTDA   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR INGRID DA CRUZ SILVA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO PATRICIA AFONSO PEDRAS(OAB: 109939/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU CASA FUNDAMENTAL EIRELI   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOR ENI DAS DORES NICACIO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO JONAS JOSE FERNANDES(OAB: 108084/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU MERCEARIA E PADARIA WM LTDA   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVOGADO FABIO JORGE BOUERE DAHER(OAB: 96158/MG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÉU SECTOR TECNOLOGIA EM SERVICOS LTDA.   </t>
   </si>
 </sst>
 </file>
@@ -1022,7 +1733,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B234"/>
+  <dimension ref="A1:B497"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1041,7 +1752,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1049,7 +1760,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1057,7 +1768,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1065,7 +1776,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1073,7 +1784,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1081,7 +1792,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1089,7 +1800,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1097,7 +1808,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1105,7 +1816,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1113,7 +1824,7 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1121,7 +1832,7 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1129,7 +1840,7 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1137,7 +1848,7 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1145,7 +1856,7 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1153,7 +1864,7 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1161,7 +1872,7 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1169,7 +1880,7 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1177,7 +1888,7 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1185,7 +1896,7 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1193,7 +1904,7 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1201,7 +1912,7 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1209,7 +1920,7 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1217,7 +1928,7 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1225,7 +1936,7 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1233,7 +1944,7 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1241,7 +1952,7 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1249,7 +1960,7 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1257,7 +1968,7 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1265,7 +1976,7 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1273,7 +1984,7 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1281,7 +1992,7 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1289,7 +2000,7 @@
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1297,7 +2008,7 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1305,7 +2016,7 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1313,7 +2024,7 @@
         <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1321,7 +2032,7 @@
         <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>76</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1329,7 +2040,7 @@
         <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1337,7 +2048,7 @@
         <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1345,7 +2056,7 @@
         <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1353,7 +2064,7 @@
         <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1361,7 +2072,7 @@
         <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1369,7 +2080,7 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1377,7 +2088,7 @@
         <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1385,7 +2096,7 @@
         <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1393,7 +2104,7 @@
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1401,7 +2112,7 @@
         <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1409,7 +2120,7 @@
         <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1417,7 +2128,7 @@
         <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>85</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1425,7 +2136,7 @@
         <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1433,7 +2144,7 @@
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>87</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1441,7 +2152,7 @@
         <v>3</v>
       </c>
       <c r="B52" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1449,7 +2160,7 @@
         <v>12</v>
       </c>
       <c r="B53" t="s">
-        <v>88</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1457,7 +2168,7 @@
         <v>12</v>
       </c>
       <c r="B54" t="s">
-        <v>89</v>
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1465,7 +2176,7 @@
         <v>12</v>
       </c>
       <c r="B55" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1473,7 +2184,7 @@
         <v>12</v>
       </c>
       <c r="B56" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1481,7 +2192,7 @@
         <v>12</v>
       </c>
       <c r="B57" t="s">
-        <v>92</v>
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1489,7 +2200,7 @@
         <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>93</v>
+        <v>138</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1497,7 +2208,7 @@
         <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1505,7 +2216,7 @@
         <v>13</v>
       </c>
       <c r="B60" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1513,7 +2224,7 @@
         <v>13</v>
       </c>
       <c r="B61" t="s">
-        <v>95</v>
+        <v>140</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1521,7 +2232,7 @@
         <v>13</v>
       </c>
       <c r="B62" t="s">
-        <v>96</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1529,7 +2240,7 @@
         <v>13</v>
       </c>
       <c r="B63" t="s">
-        <v>97</v>
+        <v>142</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1537,7 +2248,7 @@
         <v>3</v>
       </c>
       <c r="B64" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1545,7 +2256,7 @@
         <v>14</v>
       </c>
       <c r="B65" t="s">
-        <v>98</v>
+        <v>143</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1553,7 +2264,7 @@
         <v>14</v>
       </c>
       <c r="B66" t="s">
-        <v>99</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1561,7 +2272,7 @@
         <v>14</v>
       </c>
       <c r="B67" t="s">
-        <v>100</v>
+        <v>145</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1569,7 +2280,7 @@
         <v>14</v>
       </c>
       <c r="B68" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1577,7 +2288,7 @@
         <v>14</v>
       </c>
       <c r="B69" t="s">
-        <v>102</v>
+        <v>147</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1585,7 +2296,7 @@
         <v>14</v>
       </c>
       <c r="B70" t="s">
-        <v>103</v>
+        <v>148</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1593,7 +2304,7 @@
         <v>14</v>
       </c>
       <c r="B71" t="s">
-        <v>104</v>
+        <v>149</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1601,7 +2312,7 @@
         <v>14</v>
       </c>
       <c r="B72" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1609,7 +2320,7 @@
         <v>14</v>
       </c>
       <c r="B73" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1617,7 +2328,7 @@
         <v>14</v>
       </c>
       <c r="B74" t="s">
-        <v>107</v>
+        <v>152</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1625,7 +2336,7 @@
         <v>14</v>
       </c>
       <c r="B75" t="s">
-        <v>108</v>
+        <v>153</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1633,7 +2344,7 @@
         <v>14</v>
       </c>
       <c r="B76" t="s">
-        <v>109</v>
+        <v>154</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1641,7 +2352,7 @@
         <v>14</v>
       </c>
       <c r="B77" t="s">
-        <v>110</v>
+        <v>155</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1649,7 +2360,7 @@
         <v>14</v>
       </c>
       <c r="B78" t="s">
-        <v>111</v>
+        <v>156</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1657,7 +2368,7 @@
         <v>14</v>
       </c>
       <c r="B79" t="s">
-        <v>112</v>
+        <v>157</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1665,7 +2376,7 @@
         <v>14</v>
       </c>
       <c r="B80" t="s">
-        <v>113</v>
+        <v>158</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1673,7 +2384,7 @@
         <v>14</v>
       </c>
       <c r="B81" t="s">
-        <v>114</v>
+        <v>159</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1681,7 +2392,7 @@
         <v>14</v>
       </c>
       <c r="B82" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1689,7 +2400,7 @@
         <v>14</v>
       </c>
       <c r="B83" t="s">
-        <v>116</v>
+        <v>161</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1697,7 +2408,7 @@
         <v>14</v>
       </c>
       <c r="B84" t="s">
-        <v>117</v>
+        <v>162</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1705,7 +2416,7 @@
         <v>3</v>
       </c>
       <c r="B85" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1713,7 +2424,7 @@
         <v>15</v>
       </c>
       <c r="B86" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1721,7 +2432,7 @@
         <v>15</v>
       </c>
       <c r="B87" t="s">
-        <v>119</v>
+        <v>164</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1729,7 +2440,7 @@
         <v>15</v>
       </c>
       <c r="B88" t="s">
-        <v>120</v>
+        <v>165</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1737,7 +2448,7 @@
         <v>3</v>
       </c>
       <c r="B89" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1745,7 +2456,7 @@
         <v>16</v>
       </c>
       <c r="B90" t="s">
-        <v>121</v>
+        <v>166</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1753,7 +2464,7 @@
         <v>16</v>
       </c>
       <c r="B91" t="s">
-        <v>122</v>
+        <v>167</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1761,7 +2472,7 @@
         <v>16</v>
       </c>
       <c r="B92" t="s">
-        <v>123</v>
+        <v>168</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1769,7 +2480,7 @@
         <v>3</v>
       </c>
       <c r="B93" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1777,7 +2488,7 @@
         <v>17</v>
       </c>
       <c r="B94" t="s">
-        <v>124</v>
+        <v>169</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1785,7 +2496,7 @@
         <v>17</v>
       </c>
       <c r="B95" t="s">
-        <v>125</v>
+        <v>170</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1793,7 +2504,7 @@
         <v>17</v>
       </c>
       <c r="B96" t="s">
-        <v>126</v>
+        <v>171</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1801,7 +2512,7 @@
         <v>3</v>
       </c>
       <c r="B97" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1809,7 +2520,7 @@
         <v>18</v>
       </c>
       <c r="B98" t="s">
-        <v>127</v>
+        <v>172</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1817,7 +2528,7 @@
         <v>18</v>
       </c>
       <c r="B99" t="s">
-        <v>128</v>
+        <v>173</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1825,7 +2536,7 @@
         <v>18</v>
       </c>
       <c r="B100" t="s">
-        <v>129</v>
+        <v>174</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1833,7 +2544,7 @@
         <v>18</v>
       </c>
       <c r="B101" t="s">
-        <v>130</v>
+        <v>175</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1841,7 +2552,7 @@
         <v>3</v>
       </c>
       <c r="B102" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1849,7 +2560,7 @@
         <v>19</v>
       </c>
       <c r="B103" t="s">
-        <v>131</v>
+        <v>176</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1857,7 +2568,7 @@
         <v>19</v>
       </c>
       <c r="B104" t="s">
-        <v>132</v>
+        <v>177</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1865,7 +2576,7 @@
         <v>19</v>
       </c>
       <c r="B105" t="s">
-        <v>133</v>
+        <v>178</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1873,7 +2584,7 @@
         <v>19</v>
       </c>
       <c r="B106" t="s">
-        <v>134</v>
+        <v>179</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1881,7 +2592,7 @@
         <v>3</v>
       </c>
       <c r="B107" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1889,7 +2600,7 @@
         <v>20</v>
       </c>
       <c r="B108" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1897,7 +2608,7 @@
         <v>20</v>
       </c>
       <c r="B109" t="s">
-        <v>136</v>
+        <v>181</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1905,7 +2616,7 @@
         <v>20</v>
       </c>
       <c r="B110" t="s">
-        <v>137</v>
+        <v>182</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1913,7 +2624,7 @@
         <v>20</v>
       </c>
       <c r="B111" t="s">
-        <v>138</v>
+        <v>183</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1921,7 +2632,7 @@
         <v>20</v>
       </c>
       <c r="B112" t="s">
-        <v>139</v>
+        <v>184</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1929,7 +2640,7 @@
         <v>3</v>
       </c>
       <c r="B113" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1937,7 +2648,7 @@
         <v>21</v>
       </c>
       <c r="B114" t="s">
-        <v>140</v>
+        <v>185</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1945,7 +2656,7 @@
         <v>21</v>
       </c>
       <c r="B115" t="s">
-        <v>119</v>
+        <v>164</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1953,7 +2664,7 @@
         <v>21</v>
       </c>
       <c r="B116" t="s">
-        <v>141</v>
+        <v>186</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1961,7 +2672,7 @@
         <v>3</v>
       </c>
       <c r="B117" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1969,7 +2680,7 @@
         <v>22</v>
       </c>
       <c r="B118" t="s">
-        <v>142</v>
+        <v>187</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1977,7 +2688,7 @@
         <v>22</v>
       </c>
       <c r="B119" t="s">
-        <v>143</v>
+        <v>188</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1985,7 +2696,7 @@
         <v>22</v>
       </c>
       <c r="B120" t="s">
-        <v>144</v>
+        <v>189</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1993,7 +2704,7 @@
         <v>3</v>
       </c>
       <c r="B121" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2001,7 +2712,7 @@
         <v>23</v>
       </c>
       <c r="B122" t="s">
-        <v>145</v>
+        <v>190</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2009,7 +2720,7 @@
         <v>23</v>
       </c>
       <c r="B123" t="s">
-        <v>146</v>
+        <v>191</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2017,7 +2728,7 @@
         <v>23</v>
       </c>
       <c r="B124" t="s">
-        <v>147</v>
+        <v>192</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2025,7 +2736,7 @@
         <v>23</v>
       </c>
       <c r="B125" t="s">
-        <v>148</v>
+        <v>193</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -2033,7 +2744,7 @@
         <v>23</v>
       </c>
       <c r="B126" t="s">
-        <v>149</v>
+        <v>194</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -2041,7 +2752,7 @@
         <v>23</v>
       </c>
       <c r="B127" t="s">
-        <v>150</v>
+        <v>195</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2049,7 +2760,7 @@
         <v>23</v>
       </c>
       <c r="B128" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -2057,7 +2768,7 @@
         <v>3</v>
       </c>
       <c r="B129" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2065,7 +2776,7 @@
         <v>24</v>
       </c>
       <c r="B130" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2073,7 +2784,7 @@
         <v>24</v>
       </c>
       <c r="B131" t="s">
-        <v>153</v>
+        <v>198</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -2081,7 +2792,7 @@
         <v>24</v>
       </c>
       <c r="B132" t="s">
-        <v>154</v>
+        <v>199</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -2089,7 +2800,7 @@
         <v>24</v>
       </c>
       <c r="B133" t="s">
-        <v>155</v>
+        <v>200</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2097,7 +2808,7 @@
         <v>3</v>
       </c>
       <c r="B134" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -2105,7 +2816,7 @@
         <v>25</v>
       </c>
       <c r="B135" t="s">
-        <v>156</v>
+        <v>201</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -2113,7 +2824,7 @@
         <v>25</v>
       </c>
       <c r="B136" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2121,7 +2832,7 @@
         <v>25</v>
       </c>
       <c r="B137" t="s">
-        <v>158</v>
+        <v>203</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2129,7 +2840,7 @@
         <v>3</v>
       </c>
       <c r="B138" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2137,7 +2848,7 @@
         <v>26</v>
       </c>
       <c r="B139" t="s">
-        <v>159</v>
+        <v>204</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2145,7 +2856,7 @@
         <v>26</v>
       </c>
       <c r="B140" t="s">
-        <v>160</v>
+        <v>205</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2153,7 +2864,7 @@
         <v>26</v>
       </c>
       <c r="B141" t="s">
-        <v>161</v>
+        <v>206</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2161,7 +2872,7 @@
         <v>3</v>
       </c>
       <c r="B142" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2169,7 +2880,7 @@
         <v>27</v>
       </c>
       <c r="B143" t="s">
-        <v>162</v>
+        <v>207</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2177,7 +2888,7 @@
         <v>27</v>
       </c>
       <c r="B144" t="s">
-        <v>163</v>
+        <v>208</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2185,7 +2896,7 @@
         <v>27</v>
       </c>
       <c r="B145" t="s">
-        <v>164</v>
+        <v>209</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2193,7 +2904,7 @@
         <v>27</v>
       </c>
       <c r="B146" t="s">
-        <v>165</v>
+        <v>210</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2201,7 +2912,7 @@
         <v>27</v>
       </c>
       <c r="B147" t="s">
-        <v>166</v>
+        <v>211</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2209,7 +2920,7 @@
         <v>27</v>
       </c>
       <c r="B148" t="s">
-        <v>167</v>
+        <v>212</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2217,7 +2928,7 @@
         <v>3</v>
       </c>
       <c r="B149" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2225,7 +2936,7 @@
         <v>28</v>
       </c>
       <c r="B150" t="s">
-        <v>145</v>
+        <v>190</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2233,7 +2944,7 @@
         <v>28</v>
       </c>
       <c r="B151" t="s">
-        <v>146</v>
+        <v>191</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2241,7 +2952,7 @@
         <v>28</v>
       </c>
       <c r="B152" t="s">
-        <v>147</v>
+        <v>192</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -2249,7 +2960,7 @@
         <v>28</v>
       </c>
       <c r="B153" t="s">
-        <v>149</v>
+        <v>194</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -2257,7 +2968,7 @@
         <v>28</v>
       </c>
       <c r="B154" t="s">
-        <v>150</v>
+        <v>195</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -2265,7 +2976,7 @@
         <v>28</v>
       </c>
       <c r="B155" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -2273,7 +2984,7 @@
         <v>3</v>
       </c>
       <c r="B156" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -2281,7 +2992,7 @@
         <v>29</v>
       </c>
       <c r="B157" t="s">
-        <v>168</v>
+        <v>213</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -2289,7 +3000,7 @@
         <v>29</v>
       </c>
       <c r="B158" t="s">
-        <v>169</v>
+        <v>214</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -2297,7 +3008,7 @@
         <v>29</v>
       </c>
       <c r="B159" t="s">
-        <v>126</v>
+        <v>171</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -2305,7 +3016,7 @@
         <v>3</v>
       </c>
       <c r="B160" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -2313,7 +3024,7 @@
         <v>30</v>
       </c>
       <c r="B161" t="s">
-        <v>170</v>
+        <v>215</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -2321,7 +3032,7 @@
         <v>30</v>
       </c>
       <c r="B162" t="s">
-        <v>69</v>
+        <v>114</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -2329,7 +3040,7 @@
         <v>30</v>
       </c>
       <c r="B163" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -2337,7 +3048,7 @@
         <v>3</v>
       </c>
       <c r="B164" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -2345,7 +3056,7 @@
         <v>31</v>
       </c>
       <c r="B165" t="s">
-        <v>171</v>
+        <v>216</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -2353,7 +3064,7 @@
         <v>31</v>
       </c>
       <c r="B166" t="s">
-        <v>172</v>
+        <v>217</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -2361,7 +3072,7 @@
         <v>31</v>
       </c>
       <c r="B167" t="s">
-        <v>173</v>
+        <v>218</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -2369,7 +3080,7 @@
         <v>31</v>
       </c>
       <c r="B168" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -2377,7 +3088,7 @@
         <v>31</v>
       </c>
       <c r="B169" t="s">
-        <v>175</v>
+        <v>220</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -2385,7 +3096,7 @@
         <v>31</v>
       </c>
       <c r="B170" t="s">
-        <v>176</v>
+        <v>221</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -2393,7 +3104,7 @@
         <v>3</v>
       </c>
       <c r="B171" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -2401,7 +3112,7 @@
         <v>32</v>
       </c>
       <c r="B172" t="s">
-        <v>177</v>
+        <v>222</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -2409,7 +3120,7 @@
         <v>32</v>
       </c>
       <c r="B173" t="s">
-        <v>178</v>
+        <v>223</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -2417,7 +3128,7 @@
         <v>32</v>
       </c>
       <c r="B174" t="s">
-        <v>179</v>
+        <v>224</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -2425,7 +3136,7 @@
         <v>3</v>
       </c>
       <c r="B175" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -2433,7 +3144,7 @@
         <v>33</v>
       </c>
       <c r="B176" t="s">
-        <v>171</v>
+        <v>216</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -2441,7 +3152,7 @@
         <v>33</v>
       </c>
       <c r="B177" t="s">
-        <v>172</v>
+        <v>217</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -2449,7 +3160,7 @@
         <v>33</v>
       </c>
       <c r="B178" t="s">
-        <v>173</v>
+        <v>218</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -2457,7 +3168,7 @@
         <v>33</v>
       </c>
       <c r="B179" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -2465,7 +3176,7 @@
         <v>33</v>
       </c>
       <c r="B180" t="s">
-        <v>175</v>
+        <v>220</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -2473,7 +3184,7 @@
         <v>33</v>
       </c>
       <c r="B181" t="s">
-        <v>176</v>
+        <v>221</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -2481,7 +3192,7 @@
         <v>3</v>
       </c>
       <c r="B182" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -2489,7 +3200,7 @@
         <v>34</v>
       </c>
       <c r="B183" t="s">
-        <v>180</v>
+        <v>225</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -2497,7 +3208,7 @@
         <v>34</v>
       </c>
       <c r="B184" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
     </row>
     <row r="185" spans="1:2">
@@ -2505,7 +3216,7 @@
         <v>34</v>
       </c>
       <c r="B185" t="s">
-        <v>181</v>
+        <v>226</v>
       </c>
     </row>
     <row r="186" spans="1:2">
@@ -2513,7 +3224,7 @@
         <v>34</v>
       </c>
       <c r="B186" t="s">
-        <v>85</v>
+        <v>130</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -2521,7 +3232,7 @@
         <v>34</v>
       </c>
       <c r="B187" t="s">
-        <v>182</v>
+        <v>227</v>
       </c>
     </row>
     <row r="188" spans="1:2">
@@ -2529,7 +3240,7 @@
         <v>3</v>
       </c>
       <c r="B188" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -2537,7 +3248,7 @@
         <v>35</v>
       </c>
       <c r="B189" t="s">
-        <v>183</v>
+        <v>228</v>
       </c>
     </row>
     <row r="190" spans="1:2">
@@ -2545,7 +3256,7 @@
         <v>35</v>
       </c>
       <c r="B190" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -2553,7 +3264,7 @@
         <v>35</v>
       </c>
       <c r="B191" t="s">
-        <v>184</v>
+        <v>229</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -2561,7 +3272,7 @@
         <v>35</v>
       </c>
       <c r="B192" t="s">
-        <v>185</v>
+        <v>230</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -2569,7 +3280,7 @@
         <v>35</v>
       </c>
       <c r="B193" t="s">
-        <v>186</v>
+        <v>231</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -2577,7 +3288,7 @@
         <v>3</v>
       </c>
       <c r="B194" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -2585,7 +3296,7 @@
         <v>36</v>
       </c>
       <c r="B195" t="s">
-        <v>187</v>
+        <v>232</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -2593,7 +3304,7 @@
         <v>36</v>
       </c>
       <c r="B196" t="s">
-        <v>188</v>
+        <v>233</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -2601,7 +3312,7 @@
         <v>36</v>
       </c>
       <c r="B197" t="s">
-        <v>189</v>
+        <v>234</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -2609,7 +3320,7 @@
         <v>36</v>
       </c>
       <c r="B198" t="s">
-        <v>190</v>
+        <v>235</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -2617,7 +3328,7 @@
         <v>36</v>
       </c>
       <c r="B199" t="s">
-        <v>191</v>
+        <v>236</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -2625,7 +3336,7 @@
         <v>3</v>
       </c>
       <c r="B200" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -2633,7 +3344,7 @@
         <v>37</v>
       </c>
       <c r="B201" t="s">
-        <v>192</v>
+        <v>237</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -2641,7 +3352,7 @@
         <v>37</v>
       </c>
       <c r="B202" t="s">
-        <v>193</v>
+        <v>238</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -2649,7 +3360,7 @@
         <v>37</v>
       </c>
       <c r="B203" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -2657,7 +3368,7 @@
         <v>3</v>
       </c>
       <c r="B204" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -2665,7 +3376,7 @@
         <v>38</v>
       </c>
       <c r="B205" t="s">
-        <v>194</v>
+        <v>239</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -2673,7 +3384,7 @@
         <v>38</v>
       </c>
       <c r="B206" t="s">
-        <v>195</v>
+        <v>240</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -2681,7 +3392,7 @@
         <v>38</v>
       </c>
       <c r="B207" t="s">
-        <v>196</v>
+        <v>241</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -2689,7 +3400,7 @@
         <v>38</v>
       </c>
       <c r="B208" t="s">
-        <v>197</v>
+        <v>242</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -2697,7 +3408,7 @@
         <v>3</v>
       </c>
       <c r="B209" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -2705,7 +3416,7 @@
         <v>39</v>
       </c>
       <c r="B210" t="s">
-        <v>198</v>
+        <v>243</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -2713,7 +3424,7 @@
         <v>39</v>
       </c>
       <c r="B211" t="s">
-        <v>199</v>
+        <v>244</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -2721,7 +3432,7 @@
         <v>39</v>
       </c>
       <c r="B212" t="s">
-        <v>200</v>
+        <v>245</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -2729,7 +3440,7 @@
         <v>39</v>
       </c>
       <c r="B213" t="s">
-        <v>201</v>
+        <v>246</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -2737,7 +3448,7 @@
         <v>3</v>
       </c>
       <c r="B214" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="215" spans="1:2">
@@ -2745,7 +3456,7 @@
         <v>40</v>
       </c>
       <c r="B215" t="s">
-        <v>202</v>
+        <v>247</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -2753,7 +3464,7 @@
         <v>40</v>
       </c>
       <c r="B216" t="s">
-        <v>203</v>
+        <v>248</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -2761,7 +3472,7 @@
         <v>3</v>
       </c>
       <c r="B217" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="218" spans="1:2">
@@ -2769,7 +3480,7 @@
         <v>41</v>
       </c>
       <c r="B218" t="s">
-        <v>204</v>
+        <v>249</v>
       </c>
     </row>
     <row r="219" spans="1:2">
@@ -2777,7 +3488,7 @@
         <v>41</v>
       </c>
       <c r="B219" t="s">
-        <v>205</v>
+        <v>250</v>
       </c>
     </row>
     <row r="220" spans="1:2">
@@ -2785,7 +3496,7 @@
         <v>41</v>
       </c>
       <c r="B220" t="s">
-        <v>206</v>
+        <v>251</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -2793,7 +3504,7 @@
         <v>3</v>
       </c>
       <c r="B221" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="222" spans="1:2">
@@ -2801,7 +3512,7 @@
         <v>42</v>
       </c>
       <c r="B222" t="s">
-        <v>207</v>
+        <v>252</v>
       </c>
     </row>
     <row r="223" spans="1:2">
@@ -2809,7 +3520,7 @@
         <v>42</v>
       </c>
       <c r="B223" t="s">
-        <v>208</v>
+        <v>253</v>
       </c>
     </row>
     <row r="224" spans="1:2">
@@ -2817,7 +3528,7 @@
         <v>42</v>
       </c>
       <c r="B224" t="s">
-        <v>209</v>
+        <v>254</v>
       </c>
     </row>
     <row r="225" spans="1:2">
@@ -2825,7 +3536,7 @@
         <v>3</v>
       </c>
       <c r="B225" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="226" spans="1:2">
@@ -2833,7 +3544,7 @@
         <v>43</v>
       </c>
       <c r="B226" t="s">
-        <v>210</v>
+        <v>255</v>
       </c>
     </row>
     <row r="227" spans="1:2">
@@ -2841,7 +3552,7 @@
         <v>43</v>
       </c>
       <c r="B227" t="s">
-        <v>211</v>
+        <v>256</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -2849,7 +3560,7 @@
         <v>43</v>
       </c>
       <c r="B228" t="s">
-        <v>212</v>
+        <v>257</v>
       </c>
     </row>
     <row r="229" spans="1:2">
@@ -2857,7 +3568,7 @@
         <v>3</v>
       </c>
       <c r="B229" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="230" spans="1:2">
@@ -2865,7 +3576,7 @@
         <v>44</v>
       </c>
       <c r="B230" t="s">
-        <v>213</v>
+        <v>258</v>
       </c>
     </row>
     <row r="231" spans="1:2">
@@ -2873,7 +3584,7 @@
         <v>44</v>
       </c>
       <c r="B231" t="s">
-        <v>214</v>
+        <v>259</v>
       </c>
     </row>
     <row r="232" spans="1:2">
@@ -2881,7 +3592,7 @@
         <v>44</v>
       </c>
       <c r="B232" t="s">
-        <v>215</v>
+        <v>260</v>
       </c>
     </row>
     <row r="233" spans="1:2">
@@ -2889,7 +3600,7 @@
         <v>44</v>
       </c>
       <c r="B233" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
     </row>
     <row r="234" spans="1:2">
@@ -2897,7 +3608,2111 @@
         <v>3</v>
       </c>
       <c r="B234" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2">
+      <c r="A235" t="s">
+        <v>45</v>
+      </c>
+      <c r="B235" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2">
+      <c r="A236" t="s">
+        <v>45</v>
+      </c>
+      <c r="B236" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2">
+      <c r="A237" t="s">
+        <v>45</v>
+      </c>
+      <c r="B237" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2">
+      <c r="A238" t="s">
+        <v>3</v>
+      </c>
+      <c r="B238" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2">
+      <c r="A239" t="s">
+        <v>46</v>
+      </c>
+      <c r="B239" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2">
+      <c r="A240" t="s">
+        <v>46</v>
+      </c>
+      <c r="B240" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2">
+      <c r="A241" t="s">
+        <v>46</v>
+      </c>
+      <c r="B241" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2">
+      <c r="A242" t="s">
+        <v>46</v>
+      </c>
+      <c r="B242" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2">
+      <c r="A243" t="s">
+        <v>46</v>
+      </c>
+      <c r="B243" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2">
+      <c r="A244" t="s">
+        <v>46</v>
+      </c>
+      <c r="B244" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2">
+      <c r="A245" t="s">
+        <v>46</v>
+      </c>
+      <c r="B245" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2">
+      <c r="A246" t="s">
+        <v>46</v>
+      </c>
+      <c r="B246" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2">
+      <c r="A247" t="s">
+        <v>46</v>
+      </c>
+      <c r="B247" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2">
+      <c r="A248" t="s">
+        <v>46</v>
+      </c>
+      <c r="B248" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2">
+      <c r="A249" t="s">
+        <v>3</v>
+      </c>
+      <c r="B249" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2">
+      <c r="A250" t="s">
+        <v>47</v>
+      </c>
+      <c r="B250" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2">
+      <c r="A251" t="s">
+        <v>47</v>
+      </c>
+      <c r="B251" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2">
+      <c r="A252" t="s">
+        <v>47</v>
+      </c>
+      <c r="B252" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2">
+      <c r="A253" t="s">
+        <v>47</v>
+      </c>
+      <c r="B253" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2">
+      <c r="A254" t="s">
+        <v>3</v>
+      </c>
+      <c r="B254" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2">
+      <c r="A255" t="s">
+        <v>48</v>
+      </c>
+      <c r="B255" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2">
+      <c r="A256" t="s">
+        <v>48</v>
+      </c>
+      <c r="B256" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2">
+      <c r="A257" t="s">
+        <v>48</v>
+      </c>
+      <c r="B257" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2">
+      <c r="A258" t="s">
+        <v>48</v>
+      </c>
+      <c r="B258" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2">
+      <c r="A259" t="s">
+        <v>48</v>
+      </c>
+      <c r="B259" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2">
+      <c r="A260" t="s">
+        <v>3</v>
+      </c>
+      <c r="B260" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2">
+      <c r="A261" t="s">
+        <v>49</v>
+      </c>
+      <c r="B261" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2">
+      <c r="A262" t="s">
+        <v>49</v>
+      </c>
+      <c r="B262" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2">
+      <c r="A263" t="s">
+        <v>49</v>
+      </c>
+      <c r="B263" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2">
+      <c r="A264" t="s">
+        <v>3</v>
+      </c>
+      <c r="B264" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2">
+      <c r="A265" t="s">
+        <v>50</v>
+      </c>
+      <c r="B265" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2">
+      <c r="A266" t="s">
+        <v>50</v>
+      </c>
+      <c r="B266" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2">
+      <c r="A267" t="s">
+        <v>50</v>
+      </c>
+      <c r="B267" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2">
+      <c r="A268" t="s">
+        <v>50</v>
+      </c>
+      <c r="B268" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2">
+      <c r="A269" t="s">
+        <v>3</v>
+      </c>
+      <c r="B269" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2">
+      <c r="A270" t="s">
+        <v>51</v>
+      </c>
+      <c r="B270" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2">
+      <c r="A271" t="s">
+        <v>51</v>
+      </c>
+      <c r="B271" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2">
+      <c r="A272" t="s">
+        <v>51</v>
+      </c>
+      <c r="B272" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2">
+      <c r="A273" t="s">
+        <v>51</v>
+      </c>
+      <c r="B273" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2">
+      <c r="A274" t="s">
+        <v>51</v>
+      </c>
+      <c r="B274" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2">
+      <c r="A275" t="s">
+        <v>3</v>
+      </c>
+      <c r="B275" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2">
+      <c r="A276" t="s">
         <v>52</v>
+      </c>
+      <c r="B276" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2">
+      <c r="A277" t="s">
+        <v>52</v>
+      </c>
+      <c r="B277" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2">
+      <c r="A278" t="s">
+        <v>52</v>
+      </c>
+      <c r="B278" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2">
+      <c r="A279" t="s">
+        <v>52</v>
+      </c>
+      <c r="B279" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2">
+      <c r="A280" t="s">
+        <v>3</v>
+      </c>
+      <c r="B280" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2">
+      <c r="A281" t="s">
+        <v>53</v>
+      </c>
+      <c r="B281" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2">
+      <c r="A282" t="s">
+        <v>53</v>
+      </c>
+      <c r="B282" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2">
+      <c r="A283" t="s">
+        <v>53</v>
+      </c>
+      <c r="B283" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2">
+      <c r="A284" t="s">
+        <v>53</v>
+      </c>
+      <c r="B284" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2">
+      <c r="A285" t="s">
+        <v>53</v>
+      </c>
+      <c r="B285" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2">
+      <c r="A286" t="s">
+        <v>3</v>
+      </c>
+      <c r="B286" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2">
+      <c r="A287" t="s">
+        <v>54</v>
+      </c>
+      <c r="B287" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2">
+      <c r="A288" t="s">
+        <v>54</v>
+      </c>
+      <c r="B288" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2">
+      <c r="A289" t="s">
+        <v>54</v>
+      </c>
+      <c r="B289" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2">
+      <c r="A290" t="s">
+        <v>54</v>
+      </c>
+      <c r="B290" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2">
+      <c r="A291" t="s">
+        <v>54</v>
+      </c>
+      <c r="B291" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2">
+      <c r="A292" t="s">
+        <v>54</v>
+      </c>
+      <c r="B292" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2">
+      <c r="A293" t="s">
+        <v>54</v>
+      </c>
+      <c r="B293" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2">
+      <c r="A294" t="s">
+        <v>54</v>
+      </c>
+      <c r="B294" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2">
+      <c r="A295" t="s">
+        <v>54</v>
+      </c>
+      <c r="B295" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2">
+      <c r="A296" t="s">
+        <v>3</v>
+      </c>
+      <c r="B296" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2">
+      <c r="A297" t="s">
+        <v>55</v>
+      </c>
+      <c r="B297" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2">
+      <c r="A298" t="s">
+        <v>55</v>
+      </c>
+      <c r="B298" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2">
+      <c r="A299" t="s">
+        <v>55</v>
+      </c>
+      <c r="B299" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2">
+      <c r="A300" t="s">
+        <v>55</v>
+      </c>
+      <c r="B300" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2">
+      <c r="A301" t="s">
+        <v>55</v>
+      </c>
+      <c r="B301" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2">
+      <c r="A302" t="s">
+        <v>55</v>
+      </c>
+      <c r="B302" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2">
+      <c r="A303" t="s">
+        <v>55</v>
+      </c>
+      <c r="B303" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2">
+      <c r="A304" t="s">
+        <v>3</v>
+      </c>
+      <c r="B304" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2">
+      <c r="A305" t="s">
+        <v>56</v>
+      </c>
+      <c r="B305" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2">
+      <c r="A306" t="s">
+        <v>56</v>
+      </c>
+      <c r="B306" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2">
+      <c r="A307" t="s">
+        <v>56</v>
+      </c>
+      <c r="B307" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2">
+      <c r="A308" t="s">
+        <v>56</v>
+      </c>
+      <c r="B308" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2">
+      <c r="A309" t="s">
+        <v>56</v>
+      </c>
+      <c r="B309" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2">
+      <c r="A310" t="s">
+        <v>3</v>
+      </c>
+      <c r="B310" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2">
+      <c r="A311" t="s">
+        <v>57</v>
+      </c>
+      <c r="B311" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2">
+      <c r="A312" t="s">
+        <v>57</v>
+      </c>
+      <c r="B312" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2">
+      <c r="A313" t="s">
+        <v>57</v>
+      </c>
+      <c r="B313" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2">
+      <c r="A314" t="s">
+        <v>3</v>
+      </c>
+      <c r="B314" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2">
+      <c r="A315" t="s">
+        <v>58</v>
+      </c>
+      <c r="B315" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2">
+      <c r="A316" t="s">
+        <v>58</v>
+      </c>
+      <c r="B316" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2">
+      <c r="A317" t="s">
+        <v>58</v>
+      </c>
+      <c r="B317" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2">
+      <c r="A318" t="s">
+        <v>3</v>
+      </c>
+      <c r="B318" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2">
+      <c r="A319" t="s">
+        <v>59</v>
+      </c>
+      <c r="B319" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2">
+      <c r="A320" t="s">
+        <v>59</v>
+      </c>
+      <c r="B320" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2">
+      <c r="A321" t="s">
+        <v>59</v>
+      </c>
+      <c r="B321" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2">
+      <c r="A322" t="s">
+        <v>59</v>
+      </c>
+      <c r="B322" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2">
+      <c r="A323" t="s">
+        <v>3</v>
+      </c>
+      <c r="B323" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2">
+      <c r="A324" t="s">
+        <v>60</v>
+      </c>
+      <c r="B324" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2">
+      <c r="A325" t="s">
+        <v>60</v>
+      </c>
+      <c r="B325" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2">
+      <c r="A326" t="s">
+        <v>60</v>
+      </c>
+      <c r="B326" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2">
+      <c r="A327" t="s">
+        <v>60</v>
+      </c>
+      <c r="B327" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2">
+      <c r="A328" t="s">
+        <v>60</v>
+      </c>
+      <c r="B328" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2">
+      <c r="A329" t="s">
+        <v>60</v>
+      </c>
+      <c r="B329" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2">
+      <c r="A330" t="s">
+        <v>60</v>
+      </c>
+      <c r="B330" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2">
+      <c r="A331" t="s">
+        <v>60</v>
+      </c>
+      <c r="B331" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2">
+      <c r="A332" t="s">
+        <v>60</v>
+      </c>
+      <c r="B332" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2">
+      <c r="A333" t="s">
+        <v>60</v>
+      </c>
+      <c r="B333" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2">
+      <c r="A334" t="s">
+        <v>60</v>
+      </c>
+      <c r="B334" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2">
+      <c r="A335" t="s">
+        <v>60</v>
+      </c>
+      <c r="B335" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2">
+      <c r="A336" t="s">
+        <v>60</v>
+      </c>
+      <c r="B336" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2">
+      <c r="A337" t="s">
+        <v>60</v>
+      </c>
+      <c r="B337" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2">
+      <c r="A338" t="s">
+        <v>60</v>
+      </c>
+      <c r="B338" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2">
+      <c r="A339" t="s">
+        <v>60</v>
+      </c>
+      <c r="B339" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2">
+      <c r="A340" t="s">
+        <v>60</v>
+      </c>
+      <c r="B340" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2">
+      <c r="A341" t="s">
+        <v>60</v>
+      </c>
+      <c r="B341" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2">
+      <c r="A342" t="s">
+        <v>60</v>
+      </c>
+      <c r="B342" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2">
+      <c r="A343" t="s">
+        <v>3</v>
+      </c>
+      <c r="B343" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2">
+      <c r="A344" t="s">
+        <v>61</v>
+      </c>
+      <c r="B344" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2">
+      <c r="A345" t="s">
+        <v>61</v>
+      </c>
+      <c r="B345" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2">
+      <c r="A346" t="s">
+        <v>61</v>
+      </c>
+      <c r="B346" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2">
+      <c r="A347" t="s">
+        <v>61</v>
+      </c>
+      <c r="B347" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2">
+      <c r="A348" t="s">
+        <v>3</v>
+      </c>
+      <c r="B348" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2">
+      <c r="A349" t="s">
+        <v>62</v>
+      </c>
+      <c r="B349" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2">
+      <c r="A350" t="s">
+        <v>62</v>
+      </c>
+      <c r="B350" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2">
+      <c r="A351" t="s">
+        <v>62</v>
+      </c>
+      <c r="B351" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2">
+      <c r="A352" t="s">
+        <v>3</v>
+      </c>
+      <c r="B352" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2">
+      <c r="A353" t="s">
+        <v>63</v>
+      </c>
+      <c r="B353" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2">
+      <c r="A354" t="s">
+        <v>63</v>
+      </c>
+      <c r="B354" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2">
+      <c r="A355" t="s">
+        <v>63</v>
+      </c>
+      <c r="B355" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2">
+      <c r="A356" t="s">
+        <v>3</v>
+      </c>
+      <c r="B356" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2">
+      <c r="A357" t="s">
+        <v>64</v>
+      </c>
+      <c r="B357" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2">
+      <c r="A358" t="s">
+        <v>64</v>
+      </c>
+      <c r="B358" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2">
+      <c r="A359" t="s">
+        <v>64</v>
+      </c>
+      <c r="B359" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2">
+      <c r="A360" t="s">
+        <v>64</v>
+      </c>
+      <c r="B360" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2">
+      <c r="A361" t="s">
+        <v>3</v>
+      </c>
+      <c r="B361" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2">
+      <c r="A362" t="s">
+        <v>65</v>
+      </c>
+      <c r="B362" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2">
+      <c r="A363" t="s">
+        <v>65</v>
+      </c>
+      <c r="B363" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2">
+      <c r="A364" t="s">
+        <v>65</v>
+      </c>
+      <c r="B364" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2">
+      <c r="A365" t="s">
+        <v>65</v>
+      </c>
+      <c r="B365" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2">
+      <c r="A366" t="s">
+        <v>65</v>
+      </c>
+      <c r="B366" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2">
+      <c r="A367" t="s">
+        <v>65</v>
+      </c>
+      <c r="B367" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2">
+      <c r="A368" t="s">
+        <v>65</v>
+      </c>
+      <c r="B368" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2">
+      <c r="A369" t="s">
+        <v>65</v>
+      </c>
+      <c r="B369" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2">
+      <c r="A370" t="s">
+        <v>65</v>
+      </c>
+      <c r="B370" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2">
+      <c r="A371" t="s">
+        <v>65</v>
+      </c>
+      <c r="B371" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2">
+      <c r="A372" t="s">
+        <v>65</v>
+      </c>
+      <c r="B372" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2">
+      <c r="A373" t="s">
+        <v>65</v>
+      </c>
+      <c r="B373" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2">
+      <c r="A374" t="s">
+        <v>3</v>
+      </c>
+      <c r="B374" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2">
+      <c r="A375" t="s">
+        <v>66</v>
+      </c>
+      <c r="B375" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2">
+      <c r="A376" t="s">
+        <v>66</v>
+      </c>
+      <c r="B376" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2">
+      <c r="A377" t="s">
+        <v>66</v>
+      </c>
+      <c r="B377" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2">
+      <c r="A378" t="s">
+        <v>66</v>
+      </c>
+      <c r="B378" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2">
+      <c r="A379" t="s">
+        <v>3</v>
+      </c>
+      <c r="B379" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2">
+      <c r="A380" t="s">
+        <v>67</v>
+      </c>
+      <c r="B380" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2">
+      <c r="A381" t="s">
+        <v>67</v>
+      </c>
+      <c r="B381" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2">
+      <c r="A382" t="s">
+        <v>67</v>
+      </c>
+      <c r="B382" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2">
+      <c r="A383" t="s">
+        <v>67</v>
+      </c>
+      <c r="B383" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2">
+      <c r="A384" t="s">
+        <v>67</v>
+      </c>
+      <c r="B384" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2">
+      <c r="A385" t="s">
+        <v>3</v>
+      </c>
+      <c r="B385" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2">
+      <c r="A386" t="s">
+        <v>68</v>
+      </c>
+      <c r="B386" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2">
+      <c r="A387" t="s">
+        <v>68</v>
+      </c>
+      <c r="B387" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2">
+      <c r="A388" t="s">
+        <v>68</v>
+      </c>
+      <c r="B388" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2">
+      <c r="A389" t="s">
+        <v>3</v>
+      </c>
+      <c r="B389" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2">
+      <c r="A390" t="s">
+        <v>69</v>
+      </c>
+      <c r="B390" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2">
+      <c r="A391" t="s">
+        <v>69</v>
+      </c>
+      <c r="B391" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2">
+      <c r="A392" t="s">
+        <v>69</v>
+      </c>
+      <c r="B392" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2">
+      <c r="A393" t="s">
+        <v>69</v>
+      </c>
+      <c r="B393" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2">
+      <c r="A394" t="s">
+        <v>3</v>
+      </c>
+      <c r="B394" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2">
+      <c r="A395" t="s">
+        <v>70</v>
+      </c>
+      <c r="B395" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2">
+      <c r="A396" t="s">
+        <v>70</v>
+      </c>
+      <c r="B396" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2">
+      <c r="A397" t="s">
+        <v>70</v>
+      </c>
+      <c r="B397" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2">
+      <c r="A398" t="s">
+        <v>3</v>
+      </c>
+      <c r="B398" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2">
+      <c r="A399" t="s">
+        <v>71</v>
+      </c>
+      <c r="B399" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2">
+      <c r="A400" t="s">
+        <v>71</v>
+      </c>
+      <c r="B400" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2">
+      <c r="A401" t="s">
+        <v>71</v>
+      </c>
+      <c r="B401" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2">
+      <c r="A402" t="s">
+        <v>3</v>
+      </c>
+      <c r="B402" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2">
+      <c r="A403" t="s">
+        <v>72</v>
+      </c>
+      <c r="B403" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2">
+      <c r="A404" t="s">
+        <v>72</v>
+      </c>
+      <c r="B404" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2">
+      <c r="A405" t="s">
+        <v>72</v>
+      </c>
+      <c r="B405" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2">
+      <c r="A406" t="s">
+        <v>3</v>
+      </c>
+      <c r="B406" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2">
+      <c r="A407" t="s">
+        <v>73</v>
+      </c>
+      <c r="B407" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2">
+      <c r="A408" t="s">
+        <v>73</v>
+      </c>
+      <c r="B408" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2">
+      <c r="A409" t="s">
+        <v>73</v>
+      </c>
+      <c r="B409" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2">
+      <c r="A410" t="s">
+        <v>3</v>
+      </c>
+      <c r="B410" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2">
+      <c r="A411" t="s">
+        <v>74</v>
+      </c>
+      <c r="B411" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2">
+      <c r="A412" t="s">
+        <v>74</v>
+      </c>
+      <c r="B412" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2">
+      <c r="A413" t="s">
+        <v>74</v>
+      </c>
+      <c r="B413" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2">
+      <c r="A414" t="s">
+        <v>3</v>
+      </c>
+      <c r="B414" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2">
+      <c r="A415" t="s">
+        <v>75</v>
+      </c>
+      <c r="B415" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2">
+      <c r="A416" t="s">
+        <v>75</v>
+      </c>
+      <c r="B416" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2">
+      <c r="A417" t="s">
+        <v>75</v>
+      </c>
+      <c r="B417" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2">
+      <c r="A418" t="s">
+        <v>3</v>
+      </c>
+      <c r="B418" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2">
+      <c r="A419" t="s">
+        <v>76</v>
+      </c>
+      <c r="B419" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2">
+      <c r="A420" t="s">
+        <v>76</v>
+      </c>
+      <c r="B420" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2">
+      <c r="A421" t="s">
+        <v>76</v>
+      </c>
+      <c r="B421" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2">
+      <c r="A422" t="s">
+        <v>3</v>
+      </c>
+      <c r="B422" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2">
+      <c r="A423" t="s">
+        <v>77</v>
+      </c>
+      <c r="B423" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2">
+      <c r="A424" t="s">
+        <v>77</v>
+      </c>
+      <c r="B424" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2">
+      <c r="A425" t="s">
+        <v>77</v>
+      </c>
+      <c r="B425" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2">
+      <c r="A426" t="s">
+        <v>3</v>
+      </c>
+      <c r="B426" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2">
+      <c r="A427" t="s">
+        <v>78</v>
+      </c>
+      <c r="B427" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2">
+      <c r="A428" t="s">
+        <v>78</v>
+      </c>
+      <c r="B428" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="429" spans="1:2">
+      <c r="A429" t="s">
+        <v>78</v>
+      </c>
+      <c r="B429" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="430" spans="1:2">
+      <c r="A430" t="s">
+        <v>78</v>
+      </c>
+      <c r="B430" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2">
+      <c r="A431" t="s">
+        <v>3</v>
+      </c>
+      <c r="B431" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2">
+      <c r="A432" t="s">
+        <v>79</v>
+      </c>
+      <c r="B432" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2">
+      <c r="A433" t="s">
+        <v>79</v>
+      </c>
+      <c r="B433" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2">
+      <c r="A434" t="s">
+        <v>79</v>
+      </c>
+      <c r="B434" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2">
+      <c r="A435" t="s">
+        <v>79</v>
+      </c>
+      <c r="B435" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2">
+      <c r="A436" t="s">
+        <v>79</v>
+      </c>
+      <c r="B436" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2">
+      <c r="A437" t="s">
+        <v>79</v>
+      </c>
+      <c r="B437" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2">
+      <c r="A438" t="s">
+        <v>79</v>
+      </c>
+      <c r="B438" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2">
+      <c r="A439" t="s">
+        <v>79</v>
+      </c>
+      <c r="B439" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2">
+      <c r="A440" t="s">
+        <v>79</v>
+      </c>
+      <c r="B440" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2">
+      <c r="A441" t="s">
+        <v>79</v>
+      </c>
+      <c r="B441" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2">
+      <c r="A442" t="s">
+        <v>3</v>
+      </c>
+      <c r="B442" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2">
+      <c r="A443" t="s">
+        <v>80</v>
+      </c>
+      <c r="B443" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2">
+      <c r="A444" t="s">
+        <v>80</v>
+      </c>
+      <c r="B444" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2">
+      <c r="A445" t="s">
+        <v>80</v>
+      </c>
+      <c r="B445" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2">
+      <c r="A446" t="s">
+        <v>80</v>
+      </c>
+      <c r="B446" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="447" spans="1:2">
+      <c r="A447" t="s">
+        <v>3</v>
+      </c>
+      <c r="B447" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2">
+      <c r="A448" t="s">
+        <v>81</v>
+      </c>
+      <c r="B448" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2">
+      <c r="A449" t="s">
+        <v>81</v>
+      </c>
+      <c r="B449" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="450" spans="1:2">
+      <c r="A450" t="s">
+        <v>81</v>
+      </c>
+      <c r="B450" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2">
+      <c r="A451" t="s">
+        <v>81</v>
+      </c>
+      <c r="B451" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2">
+      <c r="A452" t="s">
+        <v>81</v>
+      </c>
+      <c r="B452" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="453" spans="1:2">
+      <c r="A453" t="s">
+        <v>81</v>
+      </c>
+      <c r="B453" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="454" spans="1:2">
+      <c r="A454" t="s">
+        <v>3</v>
+      </c>
+      <c r="B454" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2">
+      <c r="A455" t="s">
+        <v>82</v>
+      </c>
+      <c r="B455" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="456" spans="1:2">
+      <c r="A456" t="s">
+        <v>82</v>
+      </c>
+      <c r="B456" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="457" spans="1:2">
+      <c r="A457" t="s">
+        <v>82</v>
+      </c>
+      <c r="B457" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="458" spans="1:2">
+      <c r="A458" t="s">
+        <v>82</v>
+      </c>
+      <c r="B458" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2">
+      <c r="A459" t="s">
+        <v>82</v>
+      </c>
+      <c r="B459" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="460" spans="1:2">
+      <c r="A460" t="s">
+        <v>3</v>
+      </c>
+      <c r="B460" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="461" spans="1:2">
+      <c r="A461" t="s">
+        <v>83</v>
+      </c>
+      <c r="B461" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="462" spans="1:2">
+      <c r="A462" t="s">
+        <v>83</v>
+      </c>
+      <c r="B462" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="463" spans="1:2">
+      <c r="A463" t="s">
+        <v>83</v>
+      </c>
+      <c r="B463" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="464" spans="1:2">
+      <c r="A464" t="s">
+        <v>3</v>
+      </c>
+      <c r="B464" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2">
+      <c r="A465" t="s">
+        <v>84</v>
+      </c>
+      <c r="B465" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="466" spans="1:2">
+      <c r="A466" t="s">
+        <v>84</v>
+      </c>
+      <c r="B466" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2">
+      <c r="A467" t="s">
+        <v>84</v>
+      </c>
+      <c r="B467" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2">
+      <c r="A468" t="s">
+        <v>84</v>
+      </c>
+      <c r="B468" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="469" spans="1:2">
+      <c r="A469" t="s">
+        <v>84</v>
+      </c>
+      <c r="B469" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2">
+      <c r="A470" t="s">
+        <v>84</v>
+      </c>
+      <c r="B470" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="471" spans="1:2">
+      <c r="A471" t="s">
+        <v>84</v>
+      </c>
+      <c r="B471" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2">
+      <c r="A472" t="s">
+        <v>84</v>
+      </c>
+      <c r="B472" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2">
+      <c r="A473" t="s">
+        <v>84</v>
+      </c>
+      <c r="B473" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2">
+      <c r="A474" t="s">
+        <v>84</v>
+      </c>
+      <c r="B474" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2">
+      <c r="A475" t="s">
+        <v>84</v>
+      </c>
+      <c r="B475" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2">
+      <c r="A476" t="s">
+        <v>3</v>
+      </c>
+      <c r="B476" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="477" spans="1:2">
+      <c r="A477" t="s">
+        <v>85</v>
+      </c>
+      <c r="B477" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2">
+      <c r="A478" t="s">
+        <v>85</v>
+      </c>
+      <c r="B478" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2">
+      <c r="A479" t="s">
+        <v>85</v>
+      </c>
+      <c r="B479" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2">
+      <c r="A480" t="s">
+        <v>85</v>
+      </c>
+      <c r="B480" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="481" spans="1:2">
+      <c r="A481" t="s">
+        <v>85</v>
+      </c>
+      <c r="B481" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="482" spans="1:2">
+      <c r="A482" t="s">
+        <v>3</v>
+      </c>
+      <c r="B482" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="483" spans="1:2">
+      <c r="A483" t="s">
+        <v>86</v>
+      </c>
+      <c r="B483" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="484" spans="1:2">
+      <c r="A484" t="s">
+        <v>86</v>
+      </c>
+      <c r="B484" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="485" spans="1:2">
+      <c r="A485" t="s">
+        <v>86</v>
+      </c>
+      <c r="B485" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="486" spans="1:2">
+      <c r="A486" t="s">
+        <v>3</v>
+      </c>
+      <c r="B486" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="487" spans="1:2">
+      <c r="A487" t="s">
+        <v>87</v>
+      </c>
+      <c r="B487" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="488" spans="1:2">
+      <c r="A488" t="s">
+        <v>87</v>
+      </c>
+      <c r="B488" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="489" spans="1:2">
+      <c r="A489" t="s">
+        <v>87</v>
+      </c>
+      <c r="B489" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="490" spans="1:2">
+      <c r="A490" t="s">
+        <v>3</v>
+      </c>
+      <c r="B490" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="491" spans="1:2">
+      <c r="A491" t="s">
+        <v>88</v>
+      </c>
+      <c r="B491" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="492" spans="1:2">
+      <c r="A492" t="s">
+        <v>88</v>
+      </c>
+      <c r="B492" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="493" spans="1:2">
+      <c r="A493" t="s">
+        <v>88</v>
+      </c>
+      <c r="B493" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="494" spans="1:2">
+      <c r="A494" t="s">
+        <v>3</v>
+      </c>
+      <c r="B494" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="495" spans="1:2">
+      <c r="A495" t="s">
+        <v>89</v>
+      </c>
+      <c r="B495" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="496" spans="1:2">
+      <c r="A496" t="s">
+        <v>89</v>
+      </c>
+      <c r="B496" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="497" spans="1:2">
+      <c r="A497" t="s">
+        <v>3</v>
+      </c>
+      <c r="B497" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>